<commit_message>
TraceMap Systemtest added; Akzeptanztest 8.1-10.3
</commit_message>
<xml_diff>
--- a/Pflichtenheft/TracabilityMap.xlsx
+++ b/Pflichtenheft/TracabilityMap.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
   <si>
     <t>Anforderungen</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Use cases</t>
   </si>
   <si>
-    <t>Tests</t>
-  </si>
-  <si>
     <t>Design/Mockup</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>7. Backupsystem</t>
   </si>
   <si>
-    <t>8. 100% Übertragungs-sicherheit</t>
-  </si>
-  <si>
     <t>siehe 2.1-2.2, 2.5-2.7, 9.3</t>
   </si>
   <si>
@@ -141,12 +135,90 @@
   </si>
   <si>
     <t>3.2, 3.3</t>
+  </si>
+  <si>
+    <t>Änderung</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Versionsnummer</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <r>
+      <t>Autor des Dokuments:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Katharina Schwab</t>
+    </r>
+  </si>
+  <si>
+    <t>Dokument angelegt, Struktur festgelegt und Ucs eingetragen</t>
+  </si>
+  <si>
+    <t>MockUps eingetragen</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>Systemtest</t>
+  </si>
+  <si>
+    <t>Akzeptanztest</t>
+  </si>
+  <si>
+    <t>1-4, 14, 15</t>
+  </si>
+  <si>
+    <t>16-26,</t>
+  </si>
+  <si>
+    <t>1-4, 5-10, 13, 27-34</t>
+  </si>
+  <si>
+    <t>1-4,  5-10, 11-13,27-34</t>
+  </si>
+  <si>
+    <t>11,12,21, 22, 25-34</t>
+  </si>
+  <si>
+    <t>5-12, 16-20, 31-34,</t>
+  </si>
+  <si>
+    <t>5-12, 21-24 31-34,</t>
+  </si>
+  <si>
+    <t>16-26</t>
+  </si>
+  <si>
+    <t>8. 100%ige Übertragungs-sicherheit</t>
+  </si>
+  <si>
+    <t>MockUps angepasst, Systemtests eingetragen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="d/m/yy;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -172,7 +244,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,8 +257,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E6E6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -194,11 +278,87 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -207,6 +367,52 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -521,181 +727,335 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="C5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="4" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="D13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22"/>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="B23" s="8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="C23" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="15"/>
+      <c r="C24" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="15">
+        <v>43081</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="19">
+        <v>43082</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="9"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="13"/>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="9"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="11"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="12"/>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="9"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="13"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="12"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="10"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="9"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="13"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="12"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="14"/>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="9"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="13"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="10"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="12"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="10"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="14"/>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="9"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="13"/>
     </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
TraceMap Systemtest added, Akzeptanztest bis 10.3
</commit_message>
<xml_diff>
--- a/Pflichtenheft/TracabilityMap.xlsx
+++ b/Pflichtenheft/TracabilityMap.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
   <si>
     <t>Anforderungen</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Use cases</t>
   </si>
   <si>
-    <t>Tests</t>
-  </si>
-  <si>
     <t>Design/Mockup</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>7. Backupsystem</t>
   </si>
   <si>
-    <t>8. 100% Übertragungs-sicherheit</t>
-  </si>
-  <si>
     <t>siehe 2.1-2.2, 2.5-2.7, 9.3</t>
   </si>
   <si>
@@ -141,12 +135,90 @@
   </si>
   <si>
     <t>3.2, 3.3</t>
+  </si>
+  <si>
+    <t>Änderung</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Versionsnummer</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <r>
+      <t>Autor des Dokuments:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Katharina Schwab</t>
+    </r>
+  </si>
+  <si>
+    <t>Dokument angelegt, Struktur festgelegt und Ucs eingetragen</t>
+  </si>
+  <si>
+    <t>MockUps eingetragen</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>Systemtest</t>
+  </si>
+  <si>
+    <t>Akzeptanztest</t>
+  </si>
+  <si>
+    <t>1-4, 14, 15</t>
+  </si>
+  <si>
+    <t>16-26,</t>
+  </si>
+  <si>
+    <t>1-4, 5-10, 13, 27-34</t>
+  </si>
+  <si>
+    <t>1-4,  5-10, 11-13,27-34</t>
+  </si>
+  <si>
+    <t>11,12,21, 22, 25-34</t>
+  </si>
+  <si>
+    <t>5-12, 16-20, 31-34,</t>
+  </si>
+  <si>
+    <t>5-12, 21-24 31-34,</t>
+  </si>
+  <si>
+    <t>16-26</t>
+  </si>
+  <si>
+    <t>8. 100%ige Übertragungs-sicherheit</t>
+  </si>
+  <si>
+    <t>MockUps angepasst, Systemtests eingetragen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="d/m/yy;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -172,7 +244,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,8 +257,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E6E6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -194,11 +278,87 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -207,6 +367,52 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -521,181 +727,335 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="C5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="4" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="D13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22"/>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="B23" s="8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="C23" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="15"/>
+      <c r="C24" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="15">
+        <v>43081</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="19">
+        <v>43082</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="9"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="13"/>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="9"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="11"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="12"/>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="9"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="13"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="12"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="10"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="9"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="13"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="12"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="14"/>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="9"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="13"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="10"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="12"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="10"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="14"/>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="9"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="13"/>
     </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
ceMap Akzeptanztest added, Akzeptanztest modified
</commit_message>
<xml_diff>
--- a/Pflichtenheft/TracabilityMap.xlsx
+++ b/Pflichtenheft/TracabilityMap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t>Anforderungen</t>
   </si>
@@ -211,13 +211,58 @@
   <si>
     <t>MockUps angepasst, Systemtests eingetragen</t>
   </si>
+  <si>
+    <t>Akzeptanztest eingetragen</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1-1.5, 2.2, 9.1, 10.1, 11.1, 12.1, </t>
+  </si>
+  <si>
+    <t>4.1, 5.1, 5.2, 7.1, 15.1, 16.1</t>
+  </si>
+  <si>
+    <t>1.6-1.8, 4.1, 4.2, 5.1, 5.2, 7.1, 15.1, 16.1</t>
+  </si>
+  <si>
+    <t>1.1-1.5, 2.1, 8.1, 9.2, 10.2, 11.2, 12.1, 13.1, 13.2, 14.1</t>
+  </si>
+  <si>
+    <t>1.1-1.5, 2.1, 8.1, 8.2, 9.2, 10.3, 11.3, 12.2, 13.1, 13.2, 14.1</t>
+  </si>
+  <si>
+    <t>1.1-1.5, 2.1, 2.2, 8.1, 8.2, 9.1, 9.2, 10.1-10.3, 11.1-11.3, 12.1, 12.2, 13.1, 13.2, 14.1</t>
+  </si>
+  <si>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>8.1, 8.2, 10.1-10.3, 11.1-11.3</t>
+  </si>
+  <si>
+    <t>4.1, 5.1, 5.2, 7.1, 15.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.1, 4.2, 5.2, 7.1, 15.1, 16.1 </t>
+  </si>
+  <si>
+    <t>1.6-1.8, 7.1</t>
+  </si>
+  <si>
+    <t>2.1, 2.2</t>
+  </si>
+  <si>
+    <t>13.1, 13.2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="d/m/yy;@"/>
+    <numFmt numFmtId="164" formatCode="d/m/yy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -270,7 +315,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -354,19 +399,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -385,34 +439,57 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -729,30 +806,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="5" max="5" width="30" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>46</v>
       </c>
       <c r="E1" s="21" t="s">
@@ -760,301 +837,379 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="25"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="23" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E3" s="25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="23" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="E4" s="25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="23" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E5" s="25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="23" t="s">
         <v>49</v>
       </c>
+      <c r="E6" s="25" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="22" t="s">
         <v>12</v>
       </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="23" t="s">
         <v>52</v>
       </c>
+      <c r="E8" s="26" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="23" t="s">
         <v>54</v>
       </c>
+      <c r="E9" s="26"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="23" t="s">
         <v>53</v>
       </c>
+      <c r="E10" s="26"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="24" t="s">
         <v>35</v>
       </c>
+      <c r="D11" s="23"/>
+      <c r="E11" s="25" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="24" t="s">
         <v>28</v>
       </c>
+      <c r="C12" s="24"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="25" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="23"/>
+      <c r="C13" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="23" t="s">
         <v>55</v>
       </c>
+      <c r="E13" s="25" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="22" t="s">
         <v>19</v>
       </c>
+      <c r="B14" s="23"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="25"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="23"/>
+      <c r="C15" s="24" t="s">
         <v>35</v>
       </c>
+      <c r="D15" s="23"/>
+      <c r="E15" s="25" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="23"/>
+      <c r="C16" s="24" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="D16" s="23"/>
+      <c r="E16" s="25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="B18" s="23"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
+      <c r="B19" s="23"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C22"/>
     </row>
-    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="9" t="s">
+    <row r="24" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="11" t="s">
+      <c r="B24" s="8"/>
+      <c r="C24" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="8">
         <v>43081</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="15">
+        <v>43082</v>
+      </c>
+      <c r="C26" s="12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="19">
-        <v>43082</v>
-      </c>
-      <c r="C26" s="12" t="s">
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="14"/>
+    </row>
+    <row r="28" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="8">
+        <v>43083</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="13"/>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="11"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-      <c r="B29" s="16"/>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="9"/>
       <c r="C29" s="12"/>
     </row>
-    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="13"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="B31" s="16"/>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="14"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="9"/>
       <c r="C31" s="12"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="14"/>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="13"/>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="13"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="14"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="16"/>
+      <c r="A34" s="6"/>
+      <c r="B34" s="9"/>
       <c r="C34" s="12"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="14"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="13"/>
     </row>
     <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="9"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="13"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="14"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
-      <c r="B37" s="16"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="9"/>
       <c r="C37" s="12"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="14"/>
+      <c r="A38" s="6"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="13"/>
     </row>
     <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="9"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="13"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="E8:E10"/>
     <mergeCell ref="B37:B39"/>
     <mergeCell ref="C37:C39"/>
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="C31:C33"/>
     <mergeCell ref="B34:B36"/>
     <mergeCell ref="C34:C36"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>